<commit_message>
Updated example files for v4
</commit_message>
<xml_diff>
--- a/Documents/Examples/Devices/devices.xlsx
+++ b/Documents/Examples/Devices/devices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/temporary/devices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AF943C-4572-8B4E-8BB0-A3BF070B4E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C33333-749A-F841-9A20-C454FD98F531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17380" firstSheet="23" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="500" windowWidth="45420" windowHeight="25240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3451" uniqueCount="1339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3457" uniqueCount="1342">
   <si>
     <t>name</t>
   </si>
@@ -4093,6 +4093,15 @@
   </si>
   <si>
     <t>, Fred, Smith,</t>
+  </si>
+  <si>
+    <t>amendment</t>
+  </si>
+  <si>
+    <t>AMEND_DATE_A1</t>
+  </si>
+  <si>
+    <t>Amendment approval date</t>
   </si>
 </sst>
 </file>
@@ -4677,10 +4686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4903,6 +4912,29 @@
       </c>
       <c r="G18" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1341</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="39">
+        <v>38899</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -7470,14 +7502,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12" style="37" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="37" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
@@ -7526,8 +7558,8 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>37</v>
+      <c r="E2" s="11" t="s">
+        <v>1340</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>48</v>
@@ -15098,7 +15130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62A79FA-4693-DC4C-8533-78F85FC1D1D4}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>